<commit_message>
Todos los casos funcionando
</commit_message>
<xml_diff>
--- a/GDC_01_LegSeq_and_TargetParams.xlsx
+++ b/GDC_01_LegSeq_and_TargetParams.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\verti\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\verti\Desktop\misilnl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15807E03-DB5B-4306-9F24-5165267089B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CFBAFC1-0369-44C9-A96A-41026D4C3645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
   <si>
     <t>Step ID</t>
   </si>
@@ -423,23 +423,44 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>3 (after sequencing)</t>
   </si>
   <si>
     <t>Check that all the WPTs behind are also sequenced</t>
   </si>
   <si>
-    <t>ascendente (input5)</t>
+    <t>0.01 -&gt; 28.45</t>
+  </si>
+  <si>
+    <t>190 -&gt; 5000</t>
+  </si>
+  <si>
+    <t>18 -&gt;17</t>
+  </si>
+  <si>
+    <t>1 -&gt; 28.5</t>
+  </si>
+  <si>
+    <t>190 -&gt;4700</t>
+  </si>
+  <si>
+    <t>0.01 -&gt; 28</t>
+  </si>
+  <si>
+    <t>1 -&gt; 28</t>
+  </si>
+  <si>
+    <t>190 -&gt; 4000</t>
+  </si>
+  <si>
+    <t>4 (after REQ26)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -458,29 +479,20 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0" tint="-0.34998626667073579"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -496,6 +508,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -564,7 +582,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -587,18 +605,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -616,6 +628,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -899,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -913,20 +940,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="12" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="14"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="12"/>
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -979,13 +1006,13 @@
       <c r="C3" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="D3" s="10">
-        <v>1</v>
-      </c>
-      <c r="E3" s="10">
+      <c r="D3" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="E3" s="9">
         <v>190</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="9">
         <v>16</v>
       </c>
       <c r="G3" s="4" t="b">
@@ -1008,40 +1035,40 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" s="10">
-        <v>0</v>
-      </c>
-      <c r="E4" s="10">
-        <v>-15</v>
-      </c>
-      <c r="F4" s="10">
-        <v>22</v>
-      </c>
-      <c r="G4" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" s="4" t="s">
+      <c r="B4" s="16">
+        <v>1</v>
+      </c>
+      <c r="C4" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="20">
+        <v>1</v>
+      </c>
+      <c r="E4" s="20">
+        <v>190</v>
+      </c>
+      <c r="F4" s="20">
+        <v>16</v>
+      </c>
+      <c r="G4" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" s="2" t="s">
+      <c r="K4" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" s="18" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1055,13 +1082,13 @@
       <c r="C5" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="D5" s="10">
-        <v>1</v>
-      </c>
-      <c r="E5" s="10">
+      <c r="D5" s="9">
+        <v>1</v>
+      </c>
+      <c r="E5" s="9">
         <v>190</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="9">
         <v>16</v>
       </c>
       <c r="G5" s="4" t="b">
@@ -1093,13 +1120,13 @@
       <c r="C6" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="D6" s="10">
-        <v>1</v>
-      </c>
-      <c r="E6" s="10">
+      <c r="D6" s="9">
+        <v>1</v>
+      </c>
+      <c r="E6" s="9">
         <v>-15</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="9">
         <v>22</v>
       </c>
       <c r="G6" s="4" t="b">
@@ -1126,21 +1153,21 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="11">
-        <v>17</v>
-      </c>
-      <c r="G7" s="9" t="b">
+      <c r="F7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="8" t="b">
         <v>0</v>
       </c>
       <c r="H7" s="3" t="b">
@@ -1169,13 +1196,13 @@
       <c r="C8" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="D8" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="E8" s="10">
-        <v>190</v>
-      </c>
-      <c r="F8" s="10">
+      <c r="D8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="9">
         <v>16</v>
       </c>
       <c r="G8" s="4" t="b">
@@ -1207,13 +1234,13 @@
       <c r="C9" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="D9" s="10">
-        <v>1</v>
-      </c>
-      <c r="E9" s="10">
-        <v>190</v>
-      </c>
-      <c r="F9" s="10">
+      <c r="D9" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="9">
         <v>16</v>
       </c>
       <c r="G9" s="4" t="b">
@@ -1245,13 +1272,13 @@
       <c r="C10" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="D10" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="E10" s="10">
-        <v>190</v>
-      </c>
-      <c r="F10" s="10">
+      <c r="D10" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="9">
         <v>16</v>
       </c>
       <c r="G10" s="4" t="b">
@@ -1277,20 +1304,20 @@
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="19" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>37</v>
+      <c r="D11" s="9">
+        <v>28.45</v>
+      </c>
+      <c r="E11" s="9">
+        <v>5000</v>
+      </c>
+      <c r="F11" s="9">
+        <v>17</v>
       </c>
       <c r="G11" s="4" t="b">
         <v>0</v>
@@ -1311,27 +1338,27 @@
         <v>34</v>
       </c>
       <c r="M11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>37</v>
+      <c r="B12" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="C12" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>37</v>
+      <c r="D12" s="9">
+        <v>44.2</v>
+      </c>
+      <c r="E12" s="9">
+        <v>8000</v>
+      </c>
+      <c r="F12" s="9">
+        <v>18</v>
       </c>
       <c r="G12" s="4" t="b">
         <v>1</v>

</xml_diff>